<commit_message>
TestVINUpload.java small cleaning New3VIN_UT_SS.xlsx: VIN version changed to SYMBOL_2017
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New3VIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New3VIN_UT_SS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSAA\CODE\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="73">
   <si>
     <t>VIN</t>
   </si>
@@ -137,9 +137,6 @@
     <t>B-IMMOBILIZER/KEYLSS ENTRY/ALARM</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
     <t>Gt</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>invalidVIN</t>
   </si>
   <si>
@@ -200,7 +194,55 @@
     <t>VERSION</t>
   </si>
   <si>
-    <t>SYMBOL_2000</t>
+    <t>SYMBOL_2017</t>
+  </si>
+  <si>
+    <t>BI001</t>
+  </si>
+  <si>
+    <t>PD001</t>
+  </si>
+  <si>
+    <t>UM001</t>
+  </si>
+  <si>
+    <t>MP001</t>
+  </si>
+  <si>
+    <t>BI002</t>
+  </si>
+  <si>
+    <t>PD002</t>
+  </si>
+  <si>
+    <t>UM002</t>
+  </si>
+  <si>
+    <t>MP002</t>
+  </si>
+  <si>
+    <t>BI003</t>
+  </si>
+  <si>
+    <t>PD003</t>
+  </si>
+  <si>
+    <t>UM003</t>
+  </si>
+  <si>
+    <t>MP003</t>
+  </si>
+  <si>
+    <t>BI004</t>
+  </si>
+  <si>
+    <t>PD004</t>
+  </si>
+  <si>
+    <t>UM004</t>
+  </si>
+  <si>
+    <t>MP004</t>
   </si>
 </sst>
 </file>
@@ -558,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2:AF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -670,48 +712,48 @@
         <v>26</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>58</v>
       </c>
       <c r="C2" s="2">
         <v>2018</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>27</v>
@@ -723,19 +765,19 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O2" s="2">
         <v>8</v>
@@ -777,51 +819,51 @@
         <v>42</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="AG2" s="4">
         <v>20010101</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
         <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>58</v>
       </c>
       <c r="C3" s="2">
         <v>2018</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>27</v>
@@ -833,19 +875,19 @@
         <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="2">
         <v>8</v>
@@ -887,51 +929,51 @@
         <v>42</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="AG3" s="3">
         <v>20000101</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AJ3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
         <v>56</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
       </c>
       <c r="C4" s="2">
         <v>2018</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>27</v>
@@ -943,19 +985,19 @@
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="L4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O4" s="2">
         <v>8</v>
@@ -997,51 +1039,51 @@
         <v>42</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="AG4" s="3">
         <v>20150101</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AJ4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
         <v>56</v>
-      </c>
-      <c r="B5" t="s">
-        <v>58</v>
       </c>
       <c r="C5" s="2">
         <v>2018</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>27</v>
@@ -1053,19 +1095,19 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O5" s="2">
         <v>8</v>
@@ -1107,31 +1149,31 @@
         <v>42</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="AG5" s="3">
         <v>20190101</v>
       </c>
       <c r="AH5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AI5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AJ5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>